<commit_message>
Excel update with parameterization
</commit_message>
<xml_diff>
--- a/Modelos_conjugados.xlsx
+++ b/Modelos_conjugados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Escritorio\Bayesian_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AC6830-37CD-4BFC-9B2D-27818F191223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7984E788-346E-41DC-BE23-86F2F80624EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,31 +31,7 @@
     <author>ARLEX CASTAÑEDA</author>
   </authors>
   <commentList>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{832EF5D2-DA5F-4DDC-AC7B-CC6EA4E6A4EE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Usuario:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Se calcula internamente. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{96337DEB-5318-4A8A-A261-83A97598640C}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{96337DEB-5318-4A8A-A261-83A97598640C}">
       <text>
         <r>
           <rPr>
@@ -80,7 +56,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="1" shapeId="0" xr:uid="{DEC12DAD-039E-4AF7-916A-0B25AB264073}">
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{8A851F58-0CEB-4A8D-BAB5-33FA0CE33F9A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Usuario:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Es un slider que toma valores de 0.1 a 5 con paso de 0.1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="1" shapeId="0" xr:uid="{DEC12DAD-039E-4AF7-916A-0B25AB264073}">
       <text>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H14" authorId="1" shapeId="0" xr:uid="{B210DDB6-328D-4919-A2AA-DAB8B2A5DA6A}">
+    <comment ref="G11" authorId="1" shapeId="0" xr:uid="{B210DDB6-328D-4919-A2AA-DAB8B2A5DA6A}">
       <text>
         <r>
           <rPr>
@@ -133,57 +133,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Dist. Verosimilitud</t>
   </si>
   <si>
-    <t xml:space="preserve">Media </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varianza </t>
-  </si>
-  <si>
-    <t>Párametro_1</t>
-  </si>
-  <si>
     <t>Dist. A priori</t>
   </si>
   <si>
     <t>Normal</t>
   </si>
   <si>
-    <t>Conocida</t>
-  </si>
-  <si>
-    <t>Desconocida</t>
-  </si>
-  <si>
     <t>Ingresado por el usuario</t>
   </si>
   <si>
-    <t>Párametro_2</t>
-  </si>
-  <si>
-    <t>Párametro_3</t>
-  </si>
-  <si>
-    <t>Cant_observaciones</t>
-  </si>
-  <si>
     <t>n</t>
-  </si>
-  <si>
-    <t>Valor_1</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>Precisión (T_0 )</t>
-  </si>
-  <si>
-    <t>y_n</t>
   </si>
   <si>
     <r>
@@ -203,47 +167,6 @@
     <t>Gamma_inversa</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <r>
-      <t>desviación (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>σ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>desviación (σ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Media (y_n </t>
     </r>
@@ -258,30 +181,87 @@
     </r>
   </si>
   <si>
-    <t>Valor_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media  </t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
-    <t>Desconocida y condicionada en varianza</t>
+    <t>μ_0</t>
+  </si>
+  <si>
+    <t>CASO 1: MEDIA DESCONOCIDA Y VARIANZA CONOCIDA.</t>
+  </si>
+  <si>
+    <t>Estadístico 1</t>
   </si>
   <si>
     <r>
-      <t>σ</t>
+      <t>Varianza (σ^2</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
+        <rFont val="Calibri"/>
       </rPr>
-      <t>Ù</t>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Media muestral(y_n)</t>
+  </si>
+  <si>
+    <t>Parámetro 1</t>
+  </si>
+  <si>
+    <t>Parámetro_2</t>
+  </si>
+  <si>
+    <t>Cant.Observaciones</t>
+  </si>
+  <si>
+    <t>Parámetro 2</t>
+  </si>
+  <si>
+    <t>Parámetro 3</t>
+  </si>
+  <si>
+    <t>Desviación (t_0 )</t>
+  </si>
+  <si>
+    <t>Valor 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASO 2: MEDIA CONOCIDA Y VARIANZA DESCONOCIDA. </t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Estadístico 2</t>
+  </si>
+  <si>
+    <t>Varianza muestral (S^2)</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>β</t>
+  </si>
+  <si>
+    <t>CASO 3: MEDIA Y VARIANZA DESCONOCIDAS CON MEDIA CONDICIONADA EN LA VARIANZA.</t>
+  </si>
+  <si>
+    <t>Estimación 1</t>
+  </si>
+  <si>
+    <t>Estimación 2</t>
+  </si>
+  <si>
+    <t>Media muestral (y_n)</t>
+  </si>
+  <si>
+    <r>
+      <t>σ^</t>
     </r>
     <r>
       <rPr>
@@ -315,33 +295,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> σ_2</t>
+      <t xml:space="preserve"> σ^2</t>
     </r>
   </si>
   <si>
-    <t>μ_0</t>
-  </si>
-  <si>
-    <t>k_0</t>
-  </si>
-  <si>
-    <t>y_bar</t>
-  </si>
-  <si>
-    <t>sigma_y</t>
-  </si>
-  <si>
-    <t>Estimación_1</t>
-  </si>
-  <si>
-    <t>Estimación_2</t>
+    <t>kappa_0</t>
+  </si>
+  <si>
+    <t>α_0</t>
+  </si>
+  <si>
+    <t>β_0</t>
+  </si>
+  <si>
+    <t>Parámetro_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,8 +362,16 @@
       <family val="1"/>
       <charset val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,8 +384,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -444,15 +438,30 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,9 +469,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -477,35 +483,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -790,346 +792,280 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="5"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="F6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="16"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="2"/>
+      <c r="A7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="2"/>
+      <c r="A9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="A11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="7" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F15" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>31</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A4:XFD4"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>